<commit_message>
Changes made to test cases and test data
</commit_message>
<xml_diff>
--- a/Test_cases/Test_cases.xlsx
+++ b/Test_cases/Test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arrowelectronics-my.sharepoint.com/personal/padmakshi_jain_einfochips_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Training\Capstone P1\Caption P1\Caption-P1\Test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{A135B1C4-DE99-4C1D-B5B4-BA9DC6CB39F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{601E5E19-0D2A-4EA1-B406-0F2B63275942}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6D08DC-72F2-4E6B-A840-355F21B8ED4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EAC7F602-D227-4D4B-BEA6-3251702475A3}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{EAC7F602-D227-4D4B-BEA6-3251702475A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,11 +62,6 @@
     <t>To verify the valid record of add employee without providing credentials</t>
   </si>
   <si>
-    <t>Data 1:
-Email:princy@jain.com
-Password: padmakshi123</t>
-  </si>
-  <si>
     <t>S.No</t>
   </si>
   <si>
@@ -87,35 +82,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Data:
-1. Useremail: princy@jainemail.com
-2. Password: padmakshi123
-3. Fullname: Ken kevin
-4. Email:kevin@gmai.com
-5.Jobtitile:Engineer
-6.Selenium HQ
-</t>
-  </si>
-  <si>
     <t>User profile should be displayed on Home page</t>
-  </si>
-  <si>
-    <t>1. Navigate to the url
-2. Enter user email id
-3. Enter password
-4.Click to Directory
-5.Click to Employee
-6.Go to Edit on Ken Kevin profile
-7.Click on Contatct
-8.Enter mobile number
-9.Click on Save</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data:
-1. Useremail: princy@jainemail.com
-2. Password: padmakshi123
-3. Mobile number: 5566
-</t>
   </si>
   <si>
     <t>"Please enter a valid phone number" error message should displayed.</t>
@@ -151,14 +118,47 @@
   </si>
   <si>
     <t>Data 1:
-Useremail: saul@gmail.com
+Email:bot@behera.com
+Password: bot123</t>
+  </si>
+  <si>
+    <t>Data 1:
+Useremail: goodman@gmail.com
 Password: saul123
 Data 2:
 Useremial: kim@gmail.com
 Password: kim123
 Data 3:
-Useremial: john@gmail.com
+Useremial: wick@gmail.com
 Password: john123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data:
+1. Useremail: rohit@beheraemail.com
+2. Password: bot123
+3. Fullname: Bot Rohit
+4. Email:bot@behera.com
+5.Jobtitile:Engineer
+6.Selenium HQ
+</t>
+  </si>
+  <si>
+    <t>1. Navigate to the url
+2. Enter user email id
+3. Enter password
+4.Click to Directory
+5.Click to Employee
+6.Go to Edit on Bot Rohit profile
+7.Click on Contatct
+8.Enter mobile number
+9.Click on Save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data:
+1. Useremail: rohit@beheraemail.com
+2. Password: bot123
+3. Mobile number: 91767
+</t>
   </si>
 </sst>
 </file>
@@ -222,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -247,9 +247,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -575,7 +572,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +594,7 @@
     </row>
     <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -621,10 +618,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>5</v>
@@ -639,13 +636,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -657,13 +654,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -672,44 +669,44 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>